<commit_message>
create view for directreports
</commit_message>
<xml_diff>
--- a/CR/change requests.xlsx
+++ b/CR/change requests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80099F87-43D1-4C33-AC0C-6964A8516AC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B0592E-3386-4A8E-AF74-E2C643B8C196}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>CR</t>
   </si>
@@ -85,12 +85,27 @@
   </si>
   <si>
     <t>Edit Tables' Label</t>
+  </si>
+  <si>
+    <t>Change Navigation's List Order</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>create interface for view subordinates' 3w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(create new, assigned to me, assigned to others, my assigned to subordinate)delayed because softflow traninig at walisara </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -150,15 +165,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,45 +459,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="64.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="90.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -486,107 +511,118 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3">
-        <v>43584</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="7">
+        <v>43584</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3">
-        <v>43584</v>
-      </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="F2" s="7">
+        <v>43584</v>
+      </c>
+      <c r="G2" s="7">
+        <v>43584</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="9"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="9"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="9"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
       <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="9"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="9"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="9"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>2</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -595,19 +631,22 @@
       <c r="C11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="3">
-        <v>43584</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="7">
+        <v>43584</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="3">
-        <v>43584</v>
-      </c>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="F11" s="7">
+        <v>43584</v>
+      </c>
+      <c r="G11" s="7">
+        <v>43584</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -616,19 +655,22 @@
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="3">
-        <v>43584</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="7">
+        <v>43584</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="3">
-        <v>43584</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="F12" s="7">
+        <v>43584</v>
+      </c>
+      <c r="G12" s="7">
+        <v>43584</v>
+      </c>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
         <v>4</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -637,18 +679,174 @@
       <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="7">
+        <v>43584</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="7">
+        <v>43584</v>
+      </c>
+      <c r="G13" s="7">
+        <v>43584</v>
+      </c>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="7">
         <v>43585</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F14" s="7">
+        <v>43586</v>
+      </c>
+      <c r="G14" s="7">
+        <v>43592</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>6</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="7">
         <v>43585</v>
       </c>
-      <c r="G13" s="2"/>
+      <c r="E15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="7">
+        <v>43586</v>
+      </c>
+      <c r="G15" s="7">
+        <v>43592</v>
+      </c>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="6"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H14:H15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>